<commit_message>
EPBDS-6007 Fix conflict in method names
--HG--
branch : 5.18.x
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test/rules/functionality/Concat.xlsx
+++ b/DEV/org.openl.test/test/rules/functionality/Concat.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="119">
   <si>
     <t>Result</t>
   </si>
@@ -365,6 +365,12 @@
   </si>
   <si>
     <t>1020</t>
+  </si>
+  <si>
+    <t>10.020</t>
+  </si>
+  <si>
+    <t>1020.0</t>
   </si>
 </sst>
 </file>
@@ -527,18 +533,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="ACT_H" xfId="10"/>
@@ -826,7 +831,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -837,7 +842,7 @@
   <dimension ref="B3:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -852,9 +857,9 @@
         <v>115</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -871,7 +876,7 @@
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E5" t="s">
@@ -880,528 +885,528 @@
       <c r="F5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="5">
-        <v>30</v>
+      <c r="G5" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="5">
-        <v>30</v>
+      <c r="G6" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="5">
-        <v>30</v>
+      <c r="G7" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="5">
-        <v>30</v>
+      <c r="G8" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F9" s="1"/>
-      <c r="G9" s="5">
-        <v>30</v>
+      <c r="G9" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="4" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="5">
-        <v>30</v>
+      <c r="G10" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="4" t="s">
         <v>73</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="5">
-        <v>30</v>
+      <c r="G11" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="5">
-        <v>30</v>
+      <c r="G12" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="4" t="s">
         <v>75</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="5">
-        <v>30</v>
+      <c r="G13" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>76</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="5">
-        <v>30</v>
+      <c r="G14" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="4" t="s">
         <v>77</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="5">
-        <v>30</v>
+      <c r="G15" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="4" t="s">
         <v>78</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="5">
-        <v>30</v>
+      <c r="G16" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="4" t="s">
         <v>79</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="5">
-        <v>30</v>
+      <c r="G17" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="4" t="s">
         <v>80</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="5">
-        <v>30</v>
+      <c r="G18" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="4" t="s">
         <v>81</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="5">
-        <v>30</v>
+      <c r="G19" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="4" t="s">
         <v>82</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G20" s="5">
-        <v>30</v>
+      <c r="G20" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>83</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="5">
-        <v>30</v>
+      <c r="G21" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C22" s="4" t="s">
         <v>84</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="5">
-        <v>30</v>
+      <c r="G22" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>85</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G23" s="5">
-        <v>30</v>
+      <c r="G23" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>86</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G24" s="5">
-        <v>30</v>
+      <c r="G24" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>87</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="5">
-        <v>30</v>
+      <c r="G25" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>88</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G26" s="5">
-        <v>30</v>
+      <c r="G26" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>89</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G27" s="5">
-        <v>30</v>
+      <c r="G27" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>90</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G28" s="5">
-        <v>30</v>
+      <c r="G28" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="4" t="s">
         <v>91</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G29" s="5">
-        <v>30</v>
+      <c r="G29" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="4" t="s">
         <v>92</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="5">
-        <v>30</v>
+      <c r="G30" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="4" t="s">
         <v>93</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G31" s="5">
-        <v>30</v>
+      <c r="G31" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="4" t="s">
         <v>94</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G32" s="5">
-        <v>30</v>
+      <c r="G32" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="4" t="s">
         <v>95</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="5">
-        <v>30</v>
+      <c r="G33" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>96</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="5">
-        <v>30</v>
+      <c r="G34" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="4" t="s">
         <v>97</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G35" s="5">
-        <v>30</v>
+      <c r="G35" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>98</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>109</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="5">
-        <v>30</v>
+      <c r="G36" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>99</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>110</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="5">
-        <v>30</v>
+      <c r="G37" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="4" t="s">
         <v>100</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>111</v>
       </c>
       <c r="F38" s="1"/>
-      <c r="G38" s="5">
-        <v>30</v>
+      <c r="G38" s="5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="4" t="s">
         <v>101</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>112</v>
       </c>
       <c r="F39" s="1"/>
-      <c r="G39" s="5">
-        <v>30</v>
+      <c r="G39" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="4" t="s">
         <v>102</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>113</v>
       </c>
       <c r="F40" s="1"/>
-      <c r="G40" s="5">
-        <v>30</v>
+      <c r="G40" s="5" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>114</v>
       </c>
       <c r="F41" s="1"/>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="5" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EPBDS-6335 Move String operators to OpenL extension. The extension could be used where they are required.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.test/test/rules/functionality/Concat.xlsx
+++ b/DEV/org.openl.test/test/rules/functionality/Concat.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.test\test\rules\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16935" windowHeight="7245"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>Result</t>
   </si>
@@ -365,16 +370,25 @@
   </si>
   <si>
     <t>1020</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>org.openl.rules.binding.StringOperators.*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -546,10 +560,10 @@
     <cellStyle name="H1" xfId="7"/>
     <cellStyle name="H2" xfId="8"/>
     <cellStyle name="Heading 2 2" xfId="4"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="5"/>
     <cellStyle name="Normal 3 2" xfId="2"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 4" xfId="6"/>
     <cellStyle name="Обычный 5" xfId="3"/>
   </cellStyles>
@@ -826,7 +840,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -834,20 +848,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:G41"/>
+  <dimension ref="B3:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7">
       <c r="B3" s="1" t="s">
         <v>115</v>
       </c>
@@ -856,7 +870,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="2:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" s="1" customFormat="1">
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -867,7 +881,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -884,7 +898,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -899,7 +913,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -914,7 +928,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -929,7 +943,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -944,7 +958,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7">
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
@@ -959,7 +973,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7">
       <c r="B11" s="1" t="s">
         <v>48</v>
       </c>
@@ -974,7 +988,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7">
       <c r="B12" s="1" t="s">
         <v>49</v>
       </c>
@@ -989,7 +1003,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7">
       <c r="B13" s="1" t="s">
         <v>50</v>
       </c>
@@ -1004,7 +1018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7">
       <c r="B14" s="1" t="s">
         <v>51</v>
       </c>
@@ -1019,7 +1033,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7">
       <c r="B15" s="1" t="s">
         <v>52</v>
       </c>
@@ -1034,7 +1048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7">
       <c r="B16" s="1" t="s">
         <v>53</v>
       </c>
@@ -1049,7 +1063,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:7">
       <c r="B17" s="1" t="s">
         <v>54</v>
       </c>
@@ -1063,7 +1077,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:7">
       <c r="B18" s="1" t="s">
         <v>55</v>
       </c>
@@ -1077,7 +1091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:7">
       <c r="B19" s="1" t="s">
         <v>56</v>
       </c>
@@ -1091,7 +1105,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:7">
       <c r="B20" s="1" t="s">
         <v>57</v>
       </c>
@@ -1105,7 +1119,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7">
       <c r="B21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1119,7 +1133,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:7">
       <c r="B22" s="1" t="s">
         <v>59</v>
       </c>
@@ -1133,7 +1147,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:7">
       <c r="B23" s="1" t="s">
         <v>60</v>
       </c>
@@ -1147,7 +1161,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:7">
       <c r="B24" s="1" t="s">
         <v>61</v>
       </c>
@@ -1161,7 +1175,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:7">
       <c r="B25" s="1" t="s">
         <v>62</v>
       </c>
@@ -1175,7 +1189,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:7">
       <c r="B26" s="1" t="s">
         <v>63</v>
       </c>
@@ -1189,7 +1203,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:7">
       <c r="B27" s="1" t="s">
         <v>64</v>
       </c>
@@ -1203,7 +1217,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:7">
       <c r="B28" s="1" t="s">
         <v>65</v>
       </c>
@@ -1217,7 +1231,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:7">
       <c r="B29" s="1" t="s">
         <v>66</v>
       </c>
@@ -1231,7 +1245,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:7">
       <c r="B30" s="1" t="s">
         <v>67</v>
       </c>
@@ -1245,7 +1259,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:7">
       <c r="B31" s="1" t="s">
         <v>68</v>
       </c>
@@ -1259,7 +1273,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:7">
       <c r="B32" s="1" t="s">
         <v>69</v>
       </c>
@@ -1273,7 +1287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7">
       <c r="B33" s="1" t="s">
         <v>70</v>
       </c>
@@ -1287,7 +1301,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:7">
       <c r="B34" s="1" t="s">
         <v>71</v>
       </c>
@@ -1301,7 +1315,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7">
       <c r="B35" s="1" t="s">
         <v>72</v>
       </c>
@@ -1315,7 +1329,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:7">
       <c r="B36" s="1" t="s">
         <v>103</v>
       </c>
@@ -1330,7 +1344,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:7">
       <c r="B37" s="1" t="s">
         <v>104</v>
       </c>
@@ -1345,7 +1359,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7">
       <c r="B38" s="1" t="s">
         <v>105</v>
       </c>
@@ -1360,7 +1374,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7">
       <c r="B39" s="1" t="s">
         <v>106</v>
       </c>
@@ -1375,7 +1389,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7">
       <c r="B40" s="1" t="s">
         <v>107</v>
       </c>
@@ -1390,7 +1404,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:7">
       <c r="B41" s="1" t="s">
         <v>108</v>
       </c>
@@ -1405,8 +1419,30 @@
         <v>116</v>
       </c>
     </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C44" s="6"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B44:C44"/>
     <mergeCell ref="E3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>